<commit_message>
04.10.2020 MC Sale sDetails
</commit_message>
<xml_diff>
--- a/2020/September/Others/New folder/Active RT List of Mugdho Corporation - Copy.xlsx
+++ b/2020/September/Others/New folder/Active RT List of Mugdho Corporation - Copy.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="521">
   <si>
     <t>DEL-0179</t>
   </si>
@@ -1957,13 +1957,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomRight" activeCell="I156" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1996,7 +1997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2015,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2033,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2051,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2069,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2087,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2105,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" hidden="1">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2123,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -2140,7 +2141,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2159,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +2177,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2195,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2213,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" hidden="1">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2231,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2249,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2266,7 +2267,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -2284,7 +2285,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2303,7 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -2320,7 +2321,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2339,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2357,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2375,7 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2392,7 +2393,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -2410,7 +2411,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" hidden="1">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2428,7 +2429,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2447,7 @@
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2464,7 +2465,7 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2482,7 +2483,7 @@
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" hidden="1">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2501,7 @@
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2519,7 @@
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" hidden="1">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2536,7 +2537,7 @@
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" hidden="1">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2555,7 @@
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2572,7 +2573,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" hidden="1">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2591,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -2608,7 +2609,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" hidden="1">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2627,7 @@
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2644,7 +2645,7 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" hidden="1">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2701,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" hidden="1">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
@@ -2718,7 +2719,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" hidden="1">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +2737,7 @@
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43" s="2" t="s">
         <v>0</v>
       </c>
@@ -2754,7 +2755,7 @@
       </c>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
@@ -2772,7 +2773,7 @@
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" hidden="1">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
@@ -2790,7 +2791,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" hidden="1">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
@@ -2808,7 +2809,7 @@
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" hidden="1">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +2827,7 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" hidden="1">
       <c r="A48" s="2" t="s">
         <v>0</v>
       </c>
@@ -2844,7 +2845,7 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" hidden="1">
       <c r="A49" s="2" t="s">
         <v>0</v>
       </c>
@@ -2862,7 +2863,7 @@
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" hidden="1">
       <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +2881,7 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" hidden="1">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -2898,7 +2899,7 @@
       </c>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" hidden="1">
       <c r="A52" s="2" t="s">
         <v>0</v>
       </c>
@@ -2916,7 +2917,7 @@
       </c>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" hidden="1">
       <c r="A53" s="2" t="s">
         <v>0</v>
       </c>
@@ -2934,7 +2935,7 @@
       </c>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" hidden="1">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -2952,7 +2953,7 @@
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" hidden="1">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
@@ -2970,7 +2971,7 @@
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" hidden="1">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -2988,7 +2989,7 @@
       </c>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" hidden="1">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -3006,7 +3007,7 @@
       </c>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" hidden="1">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3025,7 @@
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" hidden="1">
       <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
@@ -3042,7 +3043,7 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" hidden="1">
       <c r="A60" s="2" t="s">
         <v>0</v>
       </c>
@@ -3060,7 +3061,7 @@
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" hidden="1">
       <c r="A61" s="2" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3079,7 @@
       </c>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" hidden="1">
       <c r="A62" s="2" t="s">
         <v>0</v>
       </c>
@@ -3096,7 +3097,7 @@
       </c>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" hidden="1">
       <c r="A63" s="2" t="s">
         <v>0</v>
       </c>
@@ -3114,7 +3115,7 @@
       </c>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" hidden="1">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -3132,7 +3133,7 @@
       </c>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65" s="2" t="s">
         <v>0</v>
       </c>
@@ -3150,7 +3151,7 @@
       </c>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" hidden="1">
       <c r="A66" s="2" t="s">
         <v>0</v>
       </c>
@@ -3168,7 +3169,7 @@
       </c>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67" s="2" t="s">
         <v>0</v>
       </c>
@@ -3186,7 +3187,7 @@
       </c>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" hidden="1">
       <c r="A68" s="2" t="s">
         <v>0</v>
       </c>
@@ -3204,7 +3205,7 @@
       </c>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" hidden="1">
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
@@ -3242,7 +3243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" hidden="1">
       <c r="A71" s="2" t="s">
         <v>0</v>
       </c>
@@ -3260,7 +3261,7 @@
       </c>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
@@ -3278,7 +3279,7 @@
       </c>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" s="2" t="s">
         <v>0</v>
       </c>
@@ -3296,7 +3297,7 @@
       </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" s="2" t="s">
         <v>0</v>
       </c>
@@ -3314,7 +3315,7 @@
       </c>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" s="2" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3333,7 @@
       </c>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76" s="2" t="s">
         <v>0</v>
       </c>
@@ -3350,7 +3351,7 @@
       </c>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
@@ -3368,7 +3369,7 @@
       </c>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78" s="2" t="s">
         <v>0</v>
       </c>
@@ -3386,7 +3387,7 @@
       </c>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79" s="2" t="s">
         <v>0</v>
       </c>
@@ -3404,7 +3405,7 @@
       </c>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" s="2" t="s">
         <v>0</v>
       </c>
@@ -3422,7 +3423,7 @@
       </c>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
@@ -3440,7 +3441,7 @@
       </c>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" hidden="1">
       <c r="A82" s="2" t="s">
         <v>0</v>
       </c>
@@ -3458,7 +3459,7 @@
       </c>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" hidden="1">
       <c r="A83" s="2" t="s">
         <v>0</v>
       </c>
@@ -3476,7 +3477,7 @@
       </c>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" hidden="1">
       <c r="A84" s="2" t="s">
         <v>0</v>
       </c>
@@ -3494,7 +3495,7 @@
       </c>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" hidden="1">
       <c r="A85" s="2" t="s">
         <v>0</v>
       </c>
@@ -3512,7 +3513,7 @@
       </c>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" hidden="1">
       <c r="A86" s="2" t="s">
         <v>0</v>
       </c>
@@ -3530,7 +3531,7 @@
       </c>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" hidden="1">
       <c r="A87" s="2" t="s">
         <v>0</v>
       </c>
@@ -3548,7 +3549,7 @@
       </c>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" hidden="1">
       <c r="A88" s="2" t="s">
         <v>0</v>
       </c>
@@ -3566,7 +3567,7 @@
       </c>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" hidden="1">
       <c r="A89" s="2" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3585,7 @@
       </c>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" hidden="1">
       <c r="A90" s="2" t="s">
         <v>0</v>
       </c>
@@ -3602,7 +3603,7 @@
       </c>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" hidden="1">
       <c r="A91" s="2" t="s">
         <v>0</v>
       </c>
@@ -3620,7 +3621,7 @@
       </c>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" hidden="1">
       <c r="A92" s="2" t="s">
         <v>0</v>
       </c>
@@ -3638,7 +3639,7 @@
       </c>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" hidden="1">
       <c r="A93" s="2" t="s">
         <v>0</v>
       </c>
@@ -3656,7 +3657,7 @@
       </c>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" hidden="1">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
@@ -3674,7 +3675,7 @@
       </c>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" hidden="1">
       <c r="A95" s="2" t="s">
         <v>0</v>
       </c>
@@ -3692,7 +3693,7 @@
       </c>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" hidden="1">
       <c r="A96" s="2" t="s">
         <v>0</v>
       </c>
@@ -3710,7 +3711,7 @@
       </c>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" hidden="1">
       <c r="A97" s="2" t="s">
         <v>0</v>
       </c>
@@ -3728,7 +3729,7 @@
       </c>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" hidden="1">
       <c r="A98" s="2" t="s">
         <v>0</v>
       </c>
@@ -3766,7 +3767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" hidden="1">
       <c r="A100" s="2" t="s">
         <v>0</v>
       </c>
@@ -3784,7 +3785,7 @@
       </c>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" hidden="1">
       <c r="A101" s="2" t="s">
         <v>0</v>
       </c>
@@ -3802,7 +3803,7 @@
       </c>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" hidden="1">
       <c r="A102" s="2" t="s">
         <v>0</v>
       </c>
@@ -3820,7 +3821,7 @@
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" hidden="1">
       <c r="A103" s="2" t="s">
         <v>0</v>
       </c>
@@ -3838,7 +3839,7 @@
       </c>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" hidden="1">
       <c r="A104" s="2" t="s">
         <v>0</v>
       </c>
@@ -3856,7 +3857,7 @@
       </c>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" hidden="1">
       <c r="A105" s="2" t="s">
         <v>0</v>
       </c>
@@ -3874,7 +3875,7 @@
       </c>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" hidden="1">
       <c r="A106" s="2" t="s">
         <v>0</v>
       </c>
@@ -3892,7 +3893,7 @@
       </c>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" hidden="1">
       <c r="A107" s="2" t="s">
         <v>0</v>
       </c>
@@ -3910,7 +3911,7 @@
       </c>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" hidden="1">
       <c r="A108" s="2" t="s">
         <v>0</v>
       </c>
@@ -3928,7 +3929,7 @@
       </c>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" hidden="1">
       <c r="A109" s="2" t="s">
         <v>0</v>
       </c>
@@ -3946,7 +3947,7 @@
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" hidden="1">
       <c r="A110" s="2" t="s">
         <v>0</v>
       </c>
@@ -3964,7 +3965,7 @@
       </c>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" hidden="1">
       <c r="A111" s="2" t="s">
         <v>0</v>
       </c>
@@ -3982,7 +3983,7 @@
       </c>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" hidden="1">
       <c r="A112" s="2" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4001,7 @@
       </c>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" hidden="1">
       <c r="A113" s="2" t="s">
         <v>0</v>
       </c>
@@ -4018,7 +4019,7 @@
       </c>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" hidden="1">
       <c r="A114" s="2" t="s">
         <v>0</v>
       </c>
@@ -4036,7 +4037,7 @@
       </c>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" hidden="1">
       <c r="A115" s="2" t="s">
         <v>0</v>
       </c>
@@ -4074,7 +4075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" hidden="1">
       <c r="A117" s="2" t="s">
         <v>0</v>
       </c>
@@ -4092,7 +4093,7 @@
       </c>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" hidden="1">
       <c r="A118" s="2" t="s">
         <v>0</v>
       </c>
@@ -4130,7 +4131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120" s="2" t="s">
         <v>0</v>
       </c>
@@ -4148,7 +4149,7 @@
       </c>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" hidden="1">
       <c r="A121" s="2" t="s">
         <v>0</v>
       </c>
@@ -4166,7 +4167,7 @@
       </c>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" hidden="1">
       <c r="A122" s="2" t="s">
         <v>0</v>
       </c>
@@ -4204,7 +4205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" hidden="1">
       <c r="A124" s="2" t="s">
         <v>0</v>
       </c>
@@ -4222,7 +4223,7 @@
       </c>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" hidden="1">
       <c r="A125" s="2" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4241,7 @@
       </c>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" hidden="1">
       <c r="A126" s="2" t="s">
         <v>0</v>
       </c>
@@ -4258,7 +4259,7 @@
       </c>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" hidden="1">
       <c r="A127" s="2" t="s">
         <v>0</v>
       </c>
@@ -4276,7 +4277,7 @@
       </c>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" hidden="1">
       <c r="A128" s="2" t="s">
         <v>0</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" hidden="1">
       <c r="A131" s="2" t="s">
         <v>0</v>
       </c>
@@ -4372,7 +4373,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" hidden="1">
       <c r="A133" s="2" t="s">
         <v>0</v>
       </c>
@@ -4390,7 +4391,7 @@
       </c>
       <c r="F133" s="3"/>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" hidden="1">
       <c r="A134" s="2" t="s">
         <v>0</v>
       </c>
@@ -4408,7 +4409,7 @@
       </c>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" hidden="1">
       <c r="A135" s="2" t="s">
         <v>0</v>
       </c>
@@ -4426,7 +4427,7 @@
       </c>
       <c r="F135" s="3"/>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" hidden="1">
       <c r="A136" s="2" t="s">
         <v>0</v>
       </c>
@@ -4444,7 +4445,7 @@
       </c>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" hidden="1">
       <c r="A137" s="2" t="s">
         <v>0</v>
       </c>
@@ -4462,7 +4463,7 @@
       </c>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" hidden="1">
       <c r="A138" s="2" t="s">
         <v>0</v>
       </c>
@@ -4480,7 +4481,7 @@
       </c>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" hidden="1">
       <c r="A139" s="2" t="s">
         <v>0</v>
       </c>
@@ -4498,7 +4499,7 @@
       </c>
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" hidden="1">
       <c r="A140" s="2" t="s">
         <v>0</v>
       </c>
@@ -4516,7 +4517,7 @@
       </c>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" hidden="1">
       <c r="A141" s="2" t="s">
         <v>0</v>
       </c>
@@ -4534,7 +4535,7 @@
       </c>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" hidden="1">
       <c r="A142" s="2" t="s">
         <v>0</v>
       </c>
@@ -4552,7 +4553,7 @@
       </c>
       <c r="F142" s="3"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" hidden="1">
       <c r="A143" s="2" t="s">
         <v>0</v>
       </c>
@@ -4570,7 +4571,7 @@
       </c>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" hidden="1">
       <c r="A144" s="2" t="s">
         <v>0</v>
       </c>
@@ -4588,7 +4589,7 @@
       </c>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" hidden="1">
       <c r="A145" s="2" t="s">
         <v>0</v>
       </c>
@@ -4606,7 +4607,7 @@
       </c>
       <c r="F145" s="3"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" hidden="1">
       <c r="A146" s="2" t="s">
         <v>0</v>
       </c>
@@ -4684,7 +4685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" hidden="1">
       <c r="A150" s="2" t="s">
         <v>0</v>
       </c>
@@ -4702,7 +4703,7 @@
       </c>
       <c r="F150" s="3"/>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" hidden="1">
       <c r="A151" s="2" t="s">
         <v>0</v>
       </c>
@@ -4720,7 +4721,7 @@
       </c>
       <c r="F151" s="3"/>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" hidden="1">
       <c r="A152" s="2" t="s">
         <v>0</v>
       </c>
@@ -4738,7 +4739,7 @@
       </c>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" hidden="1">
       <c r="A153" s="2" t="s">
         <v>0</v>
       </c>
@@ -4756,7 +4757,7 @@
       </c>
       <c r="F153" s="3"/>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" hidden="1">
       <c r="A154" s="2" t="s">
         <v>0</v>
       </c>
@@ -4774,7 +4775,7 @@
       </c>
       <c r="F154" s="3"/>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" hidden="1">
       <c r="A155" s="2" t="s">
         <v>0</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" hidden="1">
       <c r="A158" s="2" t="s">
         <v>0</v>
       </c>
@@ -4850,7 +4851,7 @@
       </c>
       <c r="F158" s="3"/>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" hidden="1">
       <c r="A159" s="2" t="s">
         <v>0</v>
       </c>
@@ -4888,7 +4889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" hidden="1">
       <c r="A161" s="2" t="s">
         <v>0</v>
       </c>
@@ -4906,7 +4907,7 @@
       </c>
       <c r="F161" s="3"/>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" hidden="1">
       <c r="A162" s="2" t="s">
         <v>0</v>
       </c>
@@ -4944,7 +4945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" hidden="1">
       <c r="A164" s="2" t="s">
         <v>0</v>
       </c>
@@ -4962,7 +4963,7 @@
       </c>
       <c r="F164" s="3"/>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" hidden="1">
       <c r="A165" s="2" t="s">
         <v>0</v>
       </c>
@@ -4980,7 +4981,7 @@
       </c>
       <c r="F165" s="3"/>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" hidden="1">
       <c r="A166" s="2" t="s">
         <v>0</v>
       </c>
@@ -4998,7 +4999,7 @@
       </c>
       <c r="F166" s="3"/>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" hidden="1">
       <c r="A167" s="2" t="s">
         <v>0</v>
       </c>
@@ -5016,7 +5017,7 @@
       </c>
       <c r="F167" s="3"/>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" hidden="1">
       <c r="A168" s="2" t="s">
         <v>0</v>
       </c>
@@ -5034,7 +5035,7 @@
       </c>
       <c r="F168" s="3"/>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" hidden="1">
       <c r="A169" s="2" t="s">
         <v>0</v>
       </c>
@@ -5052,7 +5053,7 @@
       </c>
       <c r="F169" s="3"/>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" hidden="1">
       <c r="A170" s="2" t="s">
         <v>0</v>
       </c>
@@ -5070,7 +5071,7 @@
       </c>
       <c r="F170" s="3"/>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" hidden="1">
       <c r="A171" s="2" t="s">
         <v>0</v>
       </c>
@@ -5088,7 +5089,7 @@
       </c>
       <c r="F171" s="3"/>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" hidden="1">
       <c r="A172" s="2" t="s">
         <v>0</v>
       </c>
@@ -5106,7 +5107,7 @@
       </c>
       <c r="F172" s="3"/>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" hidden="1">
       <c r="A173" s="2" t="s">
         <v>0</v>
       </c>
@@ -5124,7 +5125,7 @@
       </c>
       <c r="F173" s="3"/>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" hidden="1">
       <c r="A174" s="2" t="s">
         <v>0</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" hidden="1">
       <c r="A176" s="2" t="s">
         <v>0</v>
       </c>
@@ -5180,7 +5181,7 @@
       </c>
       <c r="F176" s="3"/>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" hidden="1">
       <c r="A177" s="2" t="s">
         <v>0</v>
       </c>
@@ -5198,7 +5199,7 @@
       </c>
       <c r="F177" s="3"/>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" hidden="1">
       <c r="A178" s="2" t="s">
         <v>0</v>
       </c>
@@ -5216,7 +5217,7 @@
       </c>
       <c r="F178" s="3"/>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" hidden="1">
       <c r="A179" s="2" t="s">
         <v>0</v>
       </c>
@@ -5234,7 +5235,7 @@
       </c>
       <c r="F179" s="3"/>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" hidden="1">
       <c r="A180" s="2" t="s">
         <v>0</v>
       </c>
@@ -5292,7 +5293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" hidden="1">
       <c r="A183" s="2" t="s">
         <v>0</v>
       </c>
@@ -5310,7 +5311,7 @@
       </c>
       <c r="F183" s="3"/>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" hidden="1">
       <c r="A184" s="2" t="s">
         <v>0</v>
       </c>
@@ -5328,7 +5329,7 @@
       </c>
       <c r="F184" s="3"/>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" hidden="1">
       <c r="A185" s="2" t="s">
         <v>0</v>
       </c>
@@ -5346,7 +5347,7 @@
       </c>
       <c r="F185" s="3"/>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" hidden="1">
       <c r="A186" s="2" t="s">
         <v>0</v>
       </c>
@@ -5364,7 +5365,7 @@
       </c>
       <c r="F186" s="3"/>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" hidden="1">
       <c r="A187" s="2" t="s">
         <v>0</v>
       </c>
@@ -5382,7 +5383,7 @@
       </c>
       <c r="F187" s="3"/>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" hidden="1">
       <c r="A188" s="2" t="s">
         <v>0</v>
       </c>
@@ -5440,7 +5441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" hidden="1">
       <c r="A191" s="2" t="s">
         <v>0</v>
       </c>
@@ -5458,7 +5459,7 @@
       </c>
       <c r="F191" s="3"/>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" hidden="1">
       <c r="A192" s="2" t="s">
         <v>0</v>
       </c>
@@ -5476,7 +5477,7 @@
       </c>
       <c r="F192" s="3"/>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" hidden="1">
       <c r="A193" s="2" t="s">
         <v>0</v>
       </c>
@@ -5494,7 +5495,7 @@
       </c>
       <c r="F193" s="3"/>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" hidden="1">
       <c r="A194" s="2" t="s">
         <v>0</v>
       </c>
@@ -5512,7 +5513,7 @@
       </c>
       <c r="F194" s="3"/>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" hidden="1">
       <c r="A195" s="2" t="s">
         <v>0</v>
       </c>
@@ -5530,7 +5531,7 @@
       </c>
       <c r="F195" s="3"/>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" hidden="1">
       <c r="A196" s="2" t="s">
         <v>0</v>
       </c>
@@ -5548,7 +5549,7 @@
       </c>
       <c r="F196" s="3"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" hidden="1">
       <c r="A197" s="2" t="s">
         <v>0</v>
       </c>
@@ -5566,7 +5567,7 @@
       </c>
       <c r="F197" s="3"/>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" hidden="1">
       <c r="A198" s="2" t="s">
         <v>0</v>
       </c>
@@ -5584,7 +5585,7 @@
       </c>
       <c r="F198" s="3"/>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" hidden="1">
       <c r="A199" s="2" t="s">
         <v>0</v>
       </c>
@@ -5602,7 +5603,7 @@
       </c>
       <c r="F199" s="3"/>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" hidden="1">
       <c r="A200" s="2" t="s">
         <v>0</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" hidden="1">
       <c r="A202" s="2" t="s">
         <v>0</v>
       </c>
@@ -5658,7 +5659,7 @@
       </c>
       <c r="F202" s="3"/>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" hidden="1">
       <c r="A203" s="2" t="s">
         <v>0</v>
       </c>
@@ -5676,7 +5677,7 @@
       </c>
       <c r="F203" s="3"/>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" hidden="1">
       <c r="A204" s="2" t="s">
         <v>0</v>
       </c>
@@ -5694,7 +5695,7 @@
       </c>
       <c r="F204" s="3"/>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" hidden="1">
       <c r="A205" s="2" t="s">
         <v>0</v>
       </c>
@@ -5712,7 +5713,7 @@
       </c>
       <c r="F205" s="3"/>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" hidden="1">
       <c r="A206" s="2" t="s">
         <v>0</v>
       </c>
@@ -5730,7 +5731,7 @@
       </c>
       <c r="F206" s="3"/>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" hidden="1">
       <c r="A207" s="2" t="s">
         <v>0</v>
       </c>
@@ -5748,7 +5749,7 @@
       </c>
       <c r="F207" s="3"/>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" hidden="1">
       <c r="A208" s="2" t="s">
         <v>0</v>
       </c>
@@ -5766,7 +5767,7 @@
       </c>
       <c r="F208" s="3"/>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" hidden="1">
       <c r="A209" s="2" t="s">
         <v>0</v>
       </c>
@@ -5784,7 +5785,7 @@
       </c>
       <c r="F209" s="3"/>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" hidden="1">
       <c r="A210" s="2" t="s">
         <v>0</v>
       </c>
@@ -5802,7 +5803,7 @@
       </c>
       <c r="F210" s="3"/>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" hidden="1">
       <c r="A211" s="2" t="s">
         <v>0</v>
       </c>
@@ -5820,7 +5821,7 @@
       </c>
       <c r="F211" s="3"/>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" hidden="1">
       <c r="A212" s="2" t="s">
         <v>0</v>
       </c>
@@ -5838,7 +5839,7 @@
       </c>
       <c r="F212" s="3"/>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" hidden="1">
       <c r="A213" s="2" t="s">
         <v>0</v>
       </c>
@@ -5856,7 +5857,7 @@
       </c>
       <c r="F213" s="3"/>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" hidden="1">
       <c r="A214" s="2" t="s">
         <v>0</v>
       </c>
@@ -5874,7 +5875,7 @@
       </c>
       <c r="F214" s="3"/>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" hidden="1">
       <c r="A215" s="2" t="s">
         <v>0</v>
       </c>
@@ -5892,7 +5893,7 @@
       </c>
       <c r="F215" s="3"/>
     </row>
-    <row r="216" spans="1:6">
+    <row r="216" spans="1:6" hidden="1">
       <c r="A216" s="2" t="s">
         <v>0</v>
       </c>
@@ -5910,7 +5911,7 @@
       </c>
       <c r="F216" s="3"/>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:6" hidden="1">
       <c r="A217" s="2" t="s">
         <v>0</v>
       </c>
@@ -5928,7 +5929,7 @@
       </c>
       <c r="F217" s="3"/>
     </row>
-    <row r="218" spans="1:6">
+    <row r="218" spans="1:6" hidden="1">
       <c r="A218" s="2" t="s">
         <v>0</v>
       </c>
@@ -6046,7 +6047,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:6">
+    <row r="224" spans="1:6" hidden="1">
       <c r="A224" s="2" t="s">
         <v>0</v>
       </c>
@@ -6064,7 +6065,7 @@
       </c>
       <c r="F224" s="3"/>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:6" hidden="1">
       <c r="A225" s="2" t="s">
         <v>0</v>
       </c>
@@ -6082,7 +6083,7 @@
       </c>
       <c r="F225" s="3"/>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:6" hidden="1">
       <c r="A226" s="2" t="s">
         <v>0</v>
       </c>
@@ -6100,7 +6101,7 @@
       </c>
       <c r="F226" s="3"/>
     </row>
-    <row r="227" spans="1:6">
+    <row r="227" spans="1:6" hidden="1">
       <c r="A227" s="2" t="s">
         <v>0</v>
       </c>
@@ -6118,7 +6119,7 @@
       </c>
       <c r="F227" s="3"/>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:6" hidden="1">
       <c r="A228" s="2" t="s">
         <v>0</v>
       </c>
@@ -6136,7 +6137,7 @@
       </c>
       <c r="F228" s="3"/>
     </row>
-    <row r="229" spans="1:6">
+    <row r="229" spans="1:6" hidden="1">
       <c r="A229" s="2" t="s">
         <v>0</v>
       </c>
@@ -6154,7 +6155,7 @@
       </c>
       <c r="F229" s="3"/>
     </row>
-    <row r="230" spans="1:6">
+    <row r="230" spans="1:6" hidden="1">
       <c r="A230" s="2" t="s">
         <v>0</v>
       </c>
@@ -6172,7 +6173,7 @@
       </c>
       <c r="F230" s="3"/>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:6" hidden="1">
       <c r="A231" s="2" t="s">
         <v>0</v>
       </c>
@@ -6190,7 +6191,7 @@
       </c>
       <c r="F231" s="3"/>
     </row>
-    <row r="232" spans="1:6">
+    <row r="232" spans="1:6" hidden="1">
       <c r="A232" s="2" t="s">
         <v>0</v>
       </c>
@@ -6208,7 +6209,7 @@
       </c>
       <c r="F232" s="3"/>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:6" hidden="1">
       <c r="A233" s="2" t="s">
         <v>0</v>
       </c>
@@ -6226,7 +6227,7 @@
       </c>
       <c r="F233" s="3"/>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:6" hidden="1">
       <c r="A234" s="2" t="s">
         <v>0</v>
       </c>
@@ -6244,7 +6245,7 @@
       </c>
       <c r="F234" s="3"/>
     </row>
-    <row r="235" spans="1:6">
+    <row r="235" spans="1:6" hidden="1">
       <c r="A235" s="2" t="s">
         <v>0</v>
       </c>
@@ -6262,7 +6263,7 @@
       </c>
       <c r="F235" s="3"/>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:6" hidden="1">
       <c r="A236" s="2" t="s">
         <v>0</v>
       </c>
@@ -6280,7 +6281,7 @@
       </c>
       <c r="F236" s="3"/>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" hidden="1">
       <c r="A237" s="2" t="s">
         <v>0</v>
       </c>
@@ -6298,7 +6299,7 @@
       </c>
       <c r="F237" s="3"/>
     </row>
-    <row r="238" spans="1:6">
+    <row r="238" spans="1:6" hidden="1">
       <c r="A238" s="2" t="s">
         <v>0</v>
       </c>
@@ -6316,7 +6317,7 @@
       </c>
       <c r="F238" s="3"/>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:6" hidden="1">
       <c r="A239" s="2" t="s">
         <v>0</v>
       </c>
@@ -6334,7 +6335,7 @@
       </c>
       <c r="F239" s="3"/>
     </row>
-    <row r="240" spans="1:6">
+    <row r="240" spans="1:6" hidden="1">
       <c r="A240" s="2" t="s">
         <v>0</v>
       </c>
@@ -6352,7 +6353,7 @@
       </c>
       <c r="F240" s="3"/>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:6" hidden="1">
       <c r="A241" s="2" t="s">
         <v>0</v>
       </c>
@@ -6370,7 +6371,7 @@
       </c>
       <c r="F241" s="3"/>
     </row>
-    <row r="242" spans="1:6">
+    <row r="242" spans="1:6" hidden="1">
       <c r="A242" s="2" t="s">
         <v>0</v>
       </c>
@@ -6388,7 +6389,7 @@
       </c>
       <c r="F242" s="3"/>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" hidden="1">
       <c r="A243" s="2" t="s">
         <v>0</v>
       </c>
@@ -6406,7 +6407,7 @@
       </c>
       <c r="F243" s="3"/>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:6" hidden="1">
       <c r="A244" s="2" t="s">
         <v>0</v>
       </c>
@@ -6424,7 +6425,7 @@
       </c>
       <c r="F244" s="3"/>
     </row>
-    <row r="245" spans="1:6">
+    <row r="245" spans="1:6" hidden="1">
       <c r="A245" s="2" t="s">
         <v>0</v>
       </c>
@@ -6442,7 +6443,7 @@
       </c>
       <c r="F245" s="3"/>
     </row>
-    <row r="246" spans="1:6">
+    <row r="246" spans="1:6" hidden="1">
       <c r="A246" s="2" t="s">
         <v>0</v>
       </c>
@@ -6456,13 +6457,11 @@
         <v>508</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F246" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="247" spans="1:6">
+      <c r="F246" s="3"/>
+    </row>
+    <row r="247" spans="1:6" hidden="1">
       <c r="A247" s="2" t="s">
         <v>0</v>
       </c>
@@ -6480,7 +6479,7 @@
       </c>
       <c r="F247" s="3"/>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:6" hidden="1">
       <c r="A248" s="2" t="s">
         <v>0</v>
       </c>
@@ -6498,7 +6497,7 @@
       </c>
       <c r="F248" s="3"/>
     </row>
-    <row r="249" spans="1:6">
+    <row r="249" spans="1:6" hidden="1">
       <c r="A249" s="2" t="s">
         <v>0</v>
       </c>
@@ -6516,7 +6515,7 @@
       </c>
       <c r="F249" s="3"/>
     </row>
-    <row r="250" spans="1:6">
+    <row r="250" spans="1:6" hidden="1">
       <c r="A250" s="2" t="s">
         <v>0</v>
       </c>
@@ -6534,7 +6533,7 @@
       </c>
       <c r="F250" s="3"/>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" hidden="1">
       <c r="A251" s="2" t="s">
         <v>0</v>
       </c>
@@ -6552,7 +6551,7 @@
       </c>
       <c r="F251" s="3"/>
     </row>
-    <row r="252" spans="1:6">
+    <row r="252" spans="1:6" hidden="1">
       <c r="A252" s="2" t="s">
         <v>0</v>
       </c>
@@ -6570,7 +6569,7 @@
       </c>
       <c r="F252" s="3"/>
     </row>
-    <row r="253" spans="1:6">
+    <row r="253" spans="1:6" hidden="1">
       <c r="A253" s="2" t="s">
         <v>0</v>
       </c>
@@ -6588,7 +6587,7 @@
       </c>
       <c r="F253" s="3"/>
     </row>
-    <row r="254" spans="1:6">
+    <row r="254" spans="1:6" hidden="1">
       <c r="A254" s="2" t="s">
         <v>0</v>
       </c>
@@ -6606,7 +6605,7 @@
       </c>
       <c r="F254" s="3"/>
     </row>
-    <row r="255" spans="1:6">
+    <row r="255" spans="1:6" hidden="1">
       <c r="A255" s="2" t="s">
         <v>0</v>
       </c>
@@ -6624,7 +6623,7 @@
       </c>
       <c r="F255" s="3"/>
     </row>
-    <row r="256" spans="1:6">
+    <row r="256" spans="1:6" hidden="1">
       <c r="A256" s="2" t="s">
         <v>0</v>
       </c>
@@ -6642,7 +6641,7 @@
       </c>
       <c r="F256" s="3"/>
     </row>
-    <row r="257" spans="1:6">
+    <row r="257" spans="1:6" hidden="1">
       <c r="A257" s="2" t="s">
         <v>0</v>
       </c>
@@ -6660,7 +6659,7 @@
       </c>
       <c r="F257" s="3"/>
     </row>
-    <row r="258" spans="1:6">
+    <row r="258" spans="1:6" hidden="1">
       <c r="A258" s="2" t="s">
         <v>0</v>
       </c>
@@ -6681,6 +6680,11 @@
   </sheetData>
   <autoFilter ref="A1:F258">
     <filterColumn colId="4"/>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>